<commit_message>
remove % from acc col
</commit_message>
<xml_diff>
--- a/logs/100c_10r_nosample/transformed/avg_results.xlsx
+++ b/logs/100c_10r_nosample/transformed/avg_results.xlsx
@@ -498,7 +498,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>60.37%</t>
+          <t>60.37</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -555,7 +555,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>60.27%</t>
+          <t>60.27</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -612,7 +612,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>59.88%</t>
+          <t>59.88</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -669,7 +669,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>60.25%</t>
+          <t>60.25</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>60.34%</t>
+          <t>60.34</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -783,7 +783,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>60.23%</t>
+          <t>60.23</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -840,7 +840,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>60.25%</t>
+          <t>60.25</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -897,7 +897,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>60.35%</t>
+          <t>60.35</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -954,7 +954,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>60.37%</t>
+          <t>60.37</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>60.49%</t>
+          <t>60.49</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">

</xml_diff>